<commit_message>
Upadted analysis with perceptions question
</commit_message>
<xml_diff>
--- a/inflation_attitudes_quantiles_discrete_q2a_agg1.xlsx
+++ b/inflation_attitudes_quantiles_discrete_q2a_agg1.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2121,6 +2121,32 @@
         <v>14.5</v>
       </c>
     </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="2">
+        <v>45748</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0.5</v>
+      </c>
+      <c r="D67">
+        <v>2.5</v>
+      </c>
+      <c r="E67">
+        <v>3.5</v>
+      </c>
+      <c r="F67">
+        <v>4.5</v>
+      </c>
+      <c r="G67">
+        <v>9.5</v>
+      </c>
+      <c r="H67">
+        <v>14.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>